<commit_message>
Changed login and password
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Valid</t>
   </si>
@@ -67,63 +67,72 @@
     <t>#</t>
   </si>
   <si>
-    <t>wellness</t>
-  </si>
-  <si>
-    <t>meredith.vanness</t>
-  </si>
-  <si>
-    <t>Meredith (Therapist and Life Coach)</t>
-  </si>
-  <si>
-    <t>https://www.balancedandwell.org/resources</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/meredith.vanness/</t>
+    <t>anxiety</t>
+  </si>
+  <si>
+    <t>anxietyocdtreatment</t>
+  </si>
+  <si>
+    <t>Amanda Petrik-Gardner, LCPC</t>
+  </si>
+  <si>
+    <t>https://linktr.ee/anxietyocd</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/anxietyocdtreatment/</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>🧠#Anxiety #OCD #BFRB Treatment
+💻Telehealth KS, CO, NE, MO, ME, MI, FL
+🖍Creator of #ocdcoloringbook on Amazon!
+📞Consultation and speaking events</t>
+  </si>
+  <si>
+    <t>neurodivergent_insights</t>
+  </si>
+  <si>
+    <t>Dr. Megan Anna Neff, Autistic-ADHD Clinician</t>
+  </si>
+  <si>
+    <t>https://linkin.bio/neurodivergent_insights</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/neurodivergent_insights/</t>
+  </si>
+  <si>
+    <t>dr</t>
+  </si>
+  <si>
+    <t>🧠 Psychology Resident &amp; author
+📖Turning academic articles into visual pixels
+🚫 No medical advice
+👇Digital downloads &amp; infographics</t>
+  </si>
+  <si>
+    <t>theanxietymd</t>
+  </si>
+  <si>
+    <t>Russell Kennedy, MD + Neuroscientist</t>
+  </si>
+  <si>
+    <t>https://linktr.ee/theanxietymd</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/theanxietymd/</t>
   </si>
   <si>
     <t>do</t>
   </si>
   <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
-    <t>〰daily quick reminders to help manage  stress, anxiety and self-doubt.
-〰helpful tips to build confidence.
-〰online options open for September ⤵</t>
-  </si>
-  <si>
-    <t>healdocumentary</t>
-  </si>
-  <si>
-    <t>HEAL Documentary 🦋</t>
-  </si>
-  <si>
-    <t>https://linktr.ee/healdocumentary</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/healdocumentary/</t>
-  </si>
-  <si>
-    <t>Documentary directed by @kellygores exploring the science &amp; spirituality behind the body's remarkable ability to HEAL. Order the companion book today!</t>
-  </si>
-  <si>
-    <t>medicalmedium</t>
-  </si>
-  <si>
-    <t>Medical Medium®</t>
-  </si>
-  <si>
-    <t>http://linktr.ee/medicalmedium</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/medicalmedium/</t>
-  </si>
-  <si>
-    <t>📚#1 NY Times Bestselling Author
-🎤Medical Medium Podcast 
-🙏🏼Helping people overcome illness 
-💚Originator of Global Celery Juice Movement</t>
+    <t>I wrote THE book on healing anxiety so you don’t have to suffer like I did.
+#1 Anxiety Physician + Somatic Intuitive.
+Get my audiobook/book here👇🏽</t>
   </si>
 </sst>
 </file>
@@ -577,7 +586,7 @@
         <v>21</v>
       </c>
       <c r="K2" s="2">
-        <v>25439</v>
+        <v>45744</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
@@ -609,16 +618,16 @@
         <v>28</v>
       </c>
       <c r="K3" s="2">
-        <v>366635</v>
+        <v>81480</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
         <v>23</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -629,25 +638,28 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2">
-        <v>4078840</v>
+        <v>33400</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
       </c>
       <c r="N4" t="s">
         <v>23</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>